<commit_message>
edited fetch implementation to send data as a form rather than inthe body for dashboard.html
</commit_message>
<xml_diff>
--- a/staticfiles/uploads/Maths_ss1_template_for_cbt.322850c44089.xlsx
+++ b/staticfiles/uploads/Maths_ss1_template_for_cbt.322850c44089.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20475" windowHeight="8355"/>
+    <workbookView windowWidth="20475" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="80">
   <si>
     <t>Mathematics</t>
   </si>
@@ -38,69 +38,207 @@
     <t>CORRECT ANSWER</t>
   </si>
   <si>
+    <t>Mensuration</t>
+  </si>
+  <si>
+    <t>what is the volume of cylinder with radius 6cm, and height 10cm</t>
+  </si>
+  <si>
+    <t>1121cm3</t>
+  </si>
+  <si>
+    <t>1000cm3</t>
+  </si>
+  <si>
+    <t>314cm3</t>
+  </si>
+  <si>
+    <t>1131cm3</t>
+  </si>
+  <si>
+    <t>a circle has a radius of 21cm. find circumference and area</t>
+  </si>
+  <si>
+    <t>c=200cm,A=138cm2</t>
+  </si>
+  <si>
+    <t>c=42cm, A=138cm2</t>
+  </si>
+  <si>
+    <t>c=100cm,150cm2</t>
+  </si>
+  <si>
+    <t>c=132cm, A=1386cm2</t>
+  </si>
+  <si>
+    <t>if 1 side of a square is 4cm, what is the area</t>
+  </si>
+  <si>
+    <t>161cm2</t>
+  </si>
+  <si>
+    <t>4cm2</t>
+  </si>
+  <si>
+    <t>8cm2</t>
+  </si>
+  <si>
+    <t>16cm2</t>
+  </si>
+  <si>
+    <t>if a cube has a length=5cm, what is area</t>
+  </si>
+  <si>
+    <t>30cm2</t>
+  </si>
+  <si>
+    <t>25cm</t>
+  </si>
+  <si>
+    <t>100cm2</t>
+  </si>
+  <si>
+    <t>150cm2</t>
+  </si>
+  <si>
+    <t>what is the perimeter of a rectangle with length 10cm, width 5cm</t>
+  </si>
+  <si>
+    <t>100cm</t>
+  </si>
+  <si>
+    <t>300cm</t>
+  </si>
+  <si>
+    <t>15cm</t>
+  </si>
+  <si>
+    <t>30cm</t>
+  </si>
+  <si>
+    <t>what is the area of a triangle with base 6cm and height 9cm</t>
+  </si>
+  <si>
+    <t>20cm</t>
+  </si>
+  <si>
+    <t>51cm</t>
+  </si>
+  <si>
+    <t>27cm</t>
+  </si>
+  <si>
+    <t>what is the circumference of a circle with diameter 15cm</t>
+  </si>
+  <si>
+    <t>40cm</t>
+  </si>
+  <si>
+    <t>47cm</t>
+  </si>
+  <si>
+    <t>what is the perimeter of an equilateral triangle of side length 9cm</t>
+  </si>
+  <si>
+    <t>9cm</t>
+  </si>
+  <si>
+    <t>18cm</t>
+  </si>
+  <si>
+    <t>what is the volume of a cube with an edge length of 9cm</t>
+  </si>
+  <si>
+    <t>900cm3</t>
+  </si>
+  <si>
+    <t>243cm3</t>
+  </si>
+  <si>
+    <t>81cm3</t>
+  </si>
+  <si>
+    <t>729cm3</t>
+  </si>
+  <si>
+    <t>what is the area of a circle with radius 10cm</t>
+  </si>
+  <si>
+    <t>10cm2</t>
+  </si>
+  <si>
+    <t>300cm2</t>
+  </si>
+  <si>
+    <t>314cm2</t>
+  </si>
+  <si>
+    <t>what is the volume of a cone with a radius of 5cm and height 8cm</t>
+  </si>
+  <si>
+    <t>158cm3</t>
+  </si>
+  <si>
+    <t>200cm3</t>
+  </si>
+  <si>
+    <t>209cm3</t>
+  </si>
+  <si>
+    <t>what is the volume of cuboid with length 8cm, width =6cm, height=4cm</t>
+  </si>
+  <si>
+    <t>182cm3</t>
+  </si>
+  <si>
+    <t>138cm3</t>
+  </si>
+  <si>
+    <t>134cm3</t>
+  </si>
+  <si>
+    <t>192cm3</t>
+  </si>
+  <si>
+    <t>if the perimeter of a square is 40cm, what is the side length</t>
+  </si>
+  <si>
+    <t>14cm</t>
+  </si>
+  <si>
+    <t>4cm</t>
+  </si>
+  <si>
+    <t>10cm</t>
+  </si>
+  <si>
+    <t>Number bases</t>
+  </si>
+  <si>
+    <t>Modular Arithmetic</t>
+  </si>
+  <si>
+    <t>Indices</t>
+  </si>
+  <si>
+    <t>Logarithms</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>Revision and welcome test</t>
+  </si>
+  <si>
+    <t>Simple Equation</t>
+  </si>
+  <si>
     <t>Variation</t>
   </si>
   <si>
-    <t>If two cups of rice cost #4, how much will 10 cups cost?</t>
-  </si>
-  <si>
     <t>Quadratic Equation</t>
   </si>
   <si>
-    <t>Quadradic equation is of the form_____</t>
-  </si>
-  <si>
-    <t>ax+b</t>
-  </si>
-  <si>
-    <t>ax+c</t>
-  </si>
-  <si>
-    <t>axb</t>
-  </si>
-  <si>
-    <t>ax2 + bx + c</t>
-  </si>
-  <si>
-    <t>Simple Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Factorize x2 + 9x + 14 </t>
-  </si>
-  <si>
-    <t>(x+2)(x-5)</t>
-  </si>
-  <si>
-    <t>(x+5)(x-4)</t>
-  </si>
-  <si>
-    <t>(x-2)(x+9)</t>
-  </si>
-  <si>
-    <t>(x+2)(x+7)</t>
-  </si>
-  <si>
-    <t>The highest power in a quadratic equation is</t>
-  </si>
-  <si>
-    <t>Number bases</t>
-  </si>
-  <si>
-    <t>Modular Arithmetic</t>
-  </si>
-  <si>
-    <t>Indices</t>
-  </si>
-  <si>
-    <t>Logarithms</t>
-  </si>
-  <si>
-    <t>Sets</t>
-  </si>
-  <si>
-    <t>Revision and welcome test</t>
-  </si>
-  <si>
     <t>Logical Reasoning</t>
   </si>
   <si>
@@ -114,9 +252,6 @@
   </si>
   <si>
     <t>Trigonometric Ratio</t>
-  </si>
-  <si>
-    <t>Mensuration</t>
   </si>
   <si>
     <t>Data presentation</t>
@@ -127,10 +262,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -171,53 +306,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,8 +396,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,29 +406,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,187 +443,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,26 +646,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,15 +711,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -608,10 +719,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -632,26 +767,26 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -660,97 +795,97 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1087,13 +1222,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="27.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="54.1428571428571" customWidth="1"/>
@@ -1139,77 +1274,257 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>40</v>
-      </c>
-      <c r="E3">
-        <v>60</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1251,92 +1566,92 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>